<commit_message>
Added some more advanced action cards
</commit_message>
<xml_diff>
--- a/Cards/Advanced Action Cards/AdvancedActions.xlsx
+++ b/Cards/Advanced Action Cards/AdvancedActions.xlsx
@@ -14,13 +14,14 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$1:$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="112">
   <si>
     <t>Number</t>
   </si>
@@ -46,18 +47,177 @@
     <t>In Unity</t>
   </si>
   <si>
+    <t>Fire Bolt</t>
+  </si>
+  <si>
+    <t>Special, Combat</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Gain a red battery to your Inventory.</t>
+  </si>
+  <si>
+    <t>Ranged Fire Attack 3.</t>
+  </si>
+  <si>
+    <t>Extreme Temperature Generator</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
+    <t>Ice Bolt</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Gain a blue battery to your Inventory.</t>
+  </si>
+  <si>
+    <t>Ranged Ice Attack 3</t>
+  </si>
+  <si>
+    <t>0°k Field Generator</t>
+  </si>
+  <si>
+    <t>Swift Bolt</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Gain a white battery to your Inventory.</t>
+  </si>
+  <si>
+    <t>Ranged Attack 4.</t>
+  </si>
+  <si>
+    <t>Accelerated Particle Generator </t>
+  </si>
+  <si>
+    <t>Crushing Bolt</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Gain a green battery to your invntory.</t>
+  </si>
+  <si>
+    <t>Siege Attack 3.</t>
+  </si>
+  <si>
+    <t>Gravity Well Generator</t>
+  </si>
+  <si>
+    <t>Ice Shield</t>
+  </si>
+  <si>
+    <t>Combat</t>
+  </si>
+  <si>
+    <t>Ice Block 3.</t>
+  </si>
+  <si>
+    <t>Ice Block 3. Reduce the armor of one enemy blocked this way by 3. Armor cannot be reduced below 1.</t>
+  </si>
+  <si>
+    <t>0°k Shielded Space Suit</t>
+  </si>
+  <si>
+    <t>Agility</t>
+  </si>
+  <si>
+    <t>Move, Combat</t>
+  </si>
+  <si>
+    <t>Move 2. During combat this turn, you may spand Move points to get Attack 1 for each.</t>
+  </si>
+  <si>
+    <t>Move 4. During combat this turn, you may spend any amount of Move points: 1 to get Attack 1 and/or 2 to get Ranged Attack 1.</t>
+  </si>
+  <si>
+    <t>Ultralight Space Suit</t>
+  </si>
+  <si>
+    <t>Intimidate</t>
+  </si>
+  <si>
+    <t>Influence, Combat</t>
+  </si>
+  <si>
+    <t>Influence 4 or Attack 3. Get Reputation -1 at the end of your turn.</t>
+  </si>
+  <si>
+    <t>Influence 8 or Attack 7. Get Reputation -2 at the end of your turn.</t>
+  </si>
+  <si>
+    <t>Song Of Wind</t>
+  </si>
+  <si>
+    <t>Move</t>
+  </si>
+  <si>
+    <t>Move 2. The Move cost of plains, deserts and wastelands is reduced by 1, to a minimum of 0 this turn.</t>
+  </si>
+  <si>
+    <t>Move 2. The Move cost of plains, deserts and wastelands is reduced by 2, to a minimum of 0.  You may pay blue energy to be able to travel through lakes for Move cost 0 this turn.</t>
+  </si>
+  <si>
+    <t>Hang-Glider Space Suit</t>
+  </si>
+  <si>
+    <t>Path Finding</t>
+  </si>
+  <si>
+    <t>Move 2. The Move cost of all terrains is reduced by 1, to a minimum of 2, this turn.</t>
+  </si>
+  <si>
+    <t>Move 4. The Move cost of all terrains is reduced to 2 this turn.</t>
+  </si>
+  <si>
+    <t>Book of Paths and Trails</t>
+  </si>
+  <si>
+    <t>Blood Ritual</t>
+  </si>
+  <si>
+    <t>Special</t>
+  </si>
+  <si>
+    <t>Take a Wound. Gain a red battery to your Inventory and an energy token of any colour.</t>
+  </si>
+  <si>
+    <t>Take a Wound. Gain three energy tokens of any colours. You may pay one energy of a basic colour to gain a battery of that colour to your Inventory.</t>
+  </si>
+  <si>
+    <t>Bio-Sciences Center Contact</t>
+  </si>
+  <si>
+    <t>Heroic Tale</t>
+  </si>
+  <si>
+    <t>Influence</t>
+  </si>
+  <si>
+    <t>Influence 3. For each Unit you recruited this turn, Reputation +1 at the end of your turn.</t>
+  </si>
+  <si>
+    <t>Influence 6, For each Unit you recruited this turn, Fame +1 and Reputation +1 at the end of your turn.</t>
+  </si>
+  <si>
+    <t>Book of Local Lore</t>
+  </si>
+  <si>
     <t>Regeneration</t>
   </si>
   <si>
     <t>Heal</t>
   </si>
   <si>
-    <t>Green</t>
-  </si>
-  <si>
     <t>Heal 1. Ready a Level 1 or 2 Unit you control.</t>
   </si>
   <si>
@@ -67,46 +227,91 @@
     <t>Mk.2 Nanobots</t>
   </si>
   <si>
+    <t>Into The Heat</t>
+  </si>
+  <si>
+    <t>Play this card at the start of combat. All of your Units get their Attack and Block values increased by 2 this combat.  You cannot assign damage to Units this turn.</t>
+  </si>
+  <si>
+    <t>Play this card at the start of the combat. All of your Units get their Attack and Block values increased by 3 this combat. You cannot assign damage to Units this turn.</t>
+  </si>
+  <si>
+    <t>Vial of Aggression Pheromones</t>
+  </si>
+  <si>
+    <t>Steady Tempo</t>
+  </si>
+  <si>
+    <t>Move 2. At the end of your turn, instead of putting this card into your discard pile, you may place it on the bottom of your Deed deck as long as it is not empty.</t>
+  </si>
+  <si>
+    <t>Move 4. At the end of your turn, instead of putting this card in your discard pile, you may place it on top of your deck.</t>
+  </si>
+  <si>
+    <t>Advanced Nutrition Supplements</t>
+  </si>
+  <si>
     <t>Diplomacy</t>
   </si>
   <si>
-    <t>Influence, Combat</t>
-  </si>
-  <si>
-    <t>White</t>
-  </si>
-  <si>
     <t>Influence 2. You may use Influence as Block this turn.</t>
   </si>
   <si>
     <t>Influence 4. Choose Ice or Fire. You may use Influence as Block for the chosen element this turn.</t>
   </si>
   <si>
-    <t>Alien Minions</t>
+    <t>Alien Linguist Contact</t>
+  </si>
+  <si>
+    <t>Decompose</t>
+  </si>
+  <si>
+    <t>When you play this card, throw away an Action card from your hand. Gain two batteries to your Inventory that are the same colour as the thrown away card.</t>
+  </si>
+  <si>
+    <t>When you play this card, throw away an Action card from your hand. Gain a battery to your Inventory of each basic color that does not match the colour of the thrown away card.</t>
+  </si>
+  <si>
+    <t>Universal Recycler</t>
+  </si>
+  <si>
+    <t>Crystal Mastery</t>
+  </si>
+  <si>
+    <t>Gain a battery to your Inventory of the same colour as a battery you already own.</t>
+  </si>
+  <si>
+    <t>At the end of the turn, any batteries you have spent this turn are returned to your Inventory.</t>
+  </si>
+  <si>
+    <t>Battery Super-Charger</t>
   </si>
   <si>
     <t>Ambush</t>
   </si>
   <si>
-    <t>Move</t>
-  </si>
-  <si>
     <t>Move 2. Add +1 to your first Attack card of any type or +2 to your first Block card of any type, whichever you play first this turn.</t>
   </si>
   <si>
     <t>Move 4. Add 2 to your first Attack card of any type or +4 to your first Block type of any type, whichever you play first this turn.</t>
   </si>
   <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>Throw away an Action card from your hand, then take a card of the same colour from the Advanced Actions offer and put it into your discard pile.</t>
+  </si>
+  <si>
+    <t>Throw away an Action card from your hand, then take a card of the same colour from the Advanced Actions offer and put it into your hand.</t>
+  </si>
+  <si>
+    <t>Flea Market Contact</t>
+  </si>
+  <si>
     <t>Ritual Attack</t>
   </si>
   <si>
-    <t>Combat</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Throw away another action card. Depending on its color, you get: Attack 5 for red, Ice Attack 3 for blue, Ranged Attack 3 for white, Siege Attack 2 for green</t>
+    <t>Throw away another action card. Depending on its color, you get: Attack 5 for red, Ice Attack 3 for blue, Ranged Attack 3 for white, Siege Attack 2 for green.</t>
   </si>
   <si>
     <t>Throw away another action card. Depending on its color, you get: Fire Attack 6 for red, Cold Fire Attack 4 for blue, Ranged Fire Attack 4 for white, Siege Fire Attack 3 for green.</t>
@@ -115,15 +320,24 @@
     <t>Junk Cannon</t>
   </si>
   <si>
+    <t>Blood of Ancients</t>
+  </si>
+  <si>
+    <t>Gain a Wound. Pay one energy of any colour. Gain a card of that colour from the Advanced Actions offer and put it into your hand.</t>
+  </si>
+  <si>
+    <t>Gain a Wound to your hand or discard pile. Use the stronger effect of any card from the Advanced Actions offer without paying its energy cost. The card remains in the offer.</t>
+  </si>
+  <si>
+    <t>Black Market Contact</t>
+  </si>
+  <si>
     <t>Temporal Portal</t>
   </si>
   <si>
     <t>Action</t>
   </si>
   <si>
-    <t>Blue</t>
-  </si>
-  <si>
     <t>Play as your action for this turn. You may move to an adjacent revealed safe space (without provoking rampaging aliens). Whether you move or not, your hand limit is higher by 1 the next time you draw cards.</t>
   </si>
   <si>
@@ -131,6 +345,18 @@
   </si>
   <si>
     <t>Spacetime Bender</t>
+  </si>
+  <si>
+    <t>Mountain Lore</t>
+  </si>
+  <si>
+    <t>Move 3. If you end your turn in hills, your Hand limit is higher by 1 the next time your draw cards.</t>
+  </si>
+  <si>
+    <t>Move 5. You can enter mountains at a Move cost of 5 and they are considered a safe space for you at the end of this turn.  If you end your turn in mountains/hills, your hand limit is higher by 2/1 the next time you draw cards.</t>
+  </si>
+  <si>
+    <t>Highlands Map</t>
   </si>
 </sst>
 </file>
@@ -145,6 +371,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -231,13 +458,16 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+      <selection pane="bottomLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2448979591837"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.7908163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,32 +500,104 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="B2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>13</v>
+      </c>
       <c r="H2" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="B3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>19</v>
+      </c>
       <c r="H3" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="B4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>24</v>
+      </c>
       <c r="H4" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="B5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>29</v>
+      </c>
       <c r="H5" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -303,23 +605,59 @@
         <v>5</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="B7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="H7" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="B8" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>39</v>
+      </c>
       <c r="H8" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -327,15 +665,33 @@
         <v>8</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>9</v>
       </c>
+      <c r="B10" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="H10" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -343,31 +699,85 @@
         <v>10</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>11</v>
       </c>
+      <c r="B12" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>48</v>
+      </c>
       <c r="H12" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>12</v>
       </c>
+      <c r="B13" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>52</v>
+      </c>
       <c r="H13" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>13</v>
       </c>
+      <c r="B14" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>57</v>
+      </c>
       <c r="H14" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -375,15 +785,33 @@
         <v>14</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
+      <c r="B16" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>62</v>
+      </c>
       <c r="H16" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -391,41 +819,77 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>13</v>
+        <v>66</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
+      <c r="B18" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>71</v>
+      </c>
       <c r="H18" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
+      <c r="B19" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>75</v>
+      </c>
       <c r="H19" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -433,25 +897,25 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>19</v>
+        <v>78</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -459,23 +923,59 @@
         <v>20</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
+      <c r="B22" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>83</v>
+      </c>
       <c r="H22" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>22</v>
       </c>
+      <c r="B23" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>87</v>
+      </c>
       <c r="H23" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -483,7 +983,7 @@
         <v>23</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -491,25 +991,25 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>24</v>
+        <v>90</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -517,7 +1017,7 @@
         <v>25</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -525,7 +1025,7 @@
         <v>26</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -533,15 +1033,33 @@
         <v>27</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>28</v>
       </c>
+      <c r="B29" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>94</v>
+      </c>
       <c r="H29" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -549,7 +1067,7 @@
         <v>29</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -557,33 +1075,51 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>28</v>
+        <v>96</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>29</v>
+        <v>97</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>31</v>
       </c>
+      <c r="B32" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>102</v>
+      </c>
       <c r="H32" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,7 +1127,7 @@
         <v>32</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -599,25 +1135,25 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>31</v>
+        <v>103</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>34</v>
+        <v>105</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>35</v>
+        <v>106</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -625,7 +1161,7 @@
         <v>34</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -633,7 +1169,7 @@
         <v>35</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -641,7 +1177,7 @@
         <v>36</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,7 +1185,7 @@
         <v>37</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -657,7 +1193,7 @@
         <v>38</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -665,15 +1201,33 @@
         <v>39</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>40</v>
       </c>
+      <c r="B41" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>111</v>
+      </c>
       <c r="H41" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -681,7 +1235,7 @@
         <v>41</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -689,7 +1243,7 @@
         <v>42</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -697,7 +1251,7 @@
         <v>43</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -705,7 +1259,7 @@
         <v>44</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -713,7 +1267,7 @@
         <v>45</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -721,7 +1275,7 @@
         <v>46</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -742,21 +1296,20 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -771,21 +1324,20 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
Finished Advanced actions spreadsheet
</commit_message>
<xml_diff>
--- a/Cards/Advanced Action Cards/AdvancedActions.xlsx
+++ b/Cards/Advanced Action Cards/AdvancedActions.xlsx
@@ -15,13 +15,15 @@
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$1:$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Sheet1!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Sheet1!$1:$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="185">
   <si>
     <t>Number</t>
   </si>
@@ -113,12 +115,24 @@
     <t>Gravity Well Generator</t>
   </si>
   <si>
+    <t>Blood Rage</t>
+  </si>
+  <si>
+    <t>Combat</t>
+  </si>
+  <si>
+    <t>Attack 2. You can take a Wound to increase this to Attack 5.</t>
+  </si>
+  <si>
+    <t>Attack 4. You can take a Wound to increase this to Attack 9.</t>
+  </si>
+  <si>
+    <t>Muscle Fibre Overdrive</t>
+  </si>
+  <si>
     <t>Ice Shield</t>
   </si>
   <si>
-    <t>Combat</t>
-  </si>
-  <si>
     <t>Ice Block 3.</t>
   </si>
   <si>
@@ -143,6 +157,21 @@
     <t>Ultralight Space Suit</t>
   </si>
   <si>
+    <t>Refreshing Walk</t>
+  </si>
+  <si>
+    <t>Move, Heal</t>
+  </si>
+  <si>
+    <t>Move 2, and Heal 1. If played during combat, Move 2 only.</t>
+  </si>
+  <si>
+    <t>Move 4 and Heal 2. If played during combat, Move 4 only.</t>
+  </si>
+  <si>
+    <t>Auto-Walking Space Suit</t>
+  </si>
+  <si>
     <t>Intimidate</t>
   </si>
   <si>
@@ -155,12 +184,24 @@
     <t>Influence 8 or Attack 7. Get Reputation -2 at the end of your turn.</t>
   </si>
   <si>
+    <t>Frost Bridge</t>
+  </si>
+  <si>
+    <t>Move</t>
+  </si>
+  <si>
+    <t>Move 2. The Move cost of swamps is reduced to 1 this turn. Moves into swamps do not provoke rampaging enemies this turn.</t>
+  </si>
+  <si>
+    <t>Move 4. You are able to travel through lakes, and the Move cost of lakes and swamps is reduced to 1 this turn. Moves into Lakes/Swamps do not provoke rampaging enemies this turn.</t>
+  </si>
+  <si>
+    <t>Amphibious Space Suit</t>
+  </si>
+  <si>
     <t>Song Of Wind</t>
   </si>
   <si>
-    <t>Move</t>
-  </si>
-  <si>
     <t>Move 2. The Move cost of plains, deserts and wastelands is reduced by 1, to a minimum of 0 this turn.</t>
   </si>
   <si>
@@ -197,6 +238,21 @@
     <t>Bio-Sciences Center Contact</t>
   </si>
   <si>
+    <t>Pure Magic</t>
+  </si>
+  <si>
+    <t>Move, Influence, Combat</t>
+  </si>
+  <si>
+    <t>When you play this, pay an energy. If you paid green, Move 4. If you paid White, Influence 4. If you paid Blue, Block 4. If you paid Red, Attack 4.</t>
+  </si>
+  <si>
+    <t>When you play this, pay an energy. If you paid green, Move 7. If you paid White, Influence 7. If you paid Blue, Block 7. If you paid Red, Attack 7.</t>
+  </si>
+  <si>
+    <t>Adaptive AI Adviser</t>
+  </si>
+  <si>
     <t>Heroic Tale</t>
   </si>
   <si>
@@ -263,6 +319,18 @@
     <t>Alien Linguist Contact</t>
   </si>
   <si>
+    <t>In Need</t>
+  </si>
+  <si>
+    <t>Influence 3. Get an additional Influence 1 for each Wound card in your hand and/or a Unit you control.</t>
+  </si>
+  <si>
+    <t>Influence 5. Get an additional Influence 2 for each Wound card in your hand and/or on a Unit you control.</t>
+  </si>
+  <si>
+    <t>Universal Empathy Translator</t>
+  </si>
+  <si>
     <t>Decompose</t>
   </si>
   <si>
@@ -287,6 +355,18 @@
     <t>Battery Super-Charger</t>
   </si>
   <si>
+    <t>Mana Storm</t>
+  </si>
+  <si>
+    <t>Choose an energy die in the Source that is showing a basic colour. Gain a battery of that colour to your Inventory, then immediately reroll that die and return it to the Source.</t>
+  </si>
+  <si>
+    <t>Re-roll all dice in the Source. You can use three extra dice from the Source, and you can use dice showing black or gold as energy of any basic colour, regardless of the Round.</t>
+  </si>
+  <si>
+    <t>Energy Storm</t>
+  </si>
+  <si>
     <t>Ambush</t>
   </si>
   <si>
@@ -296,6 +376,48 @@
     <t>Move 4. Add 2 to your first Attack card of any type or +4 to your first Block type of any type, whichever you play first this turn.</t>
   </si>
   <si>
+    <t>Camouflaged Space Suit</t>
+  </si>
+  <si>
+    <t>Maximal Effect</t>
+  </si>
+  <si>
+    <t>When you play this, throw away another Action card from your hand. Use the basic effect of that card 3 times.</t>
+  </si>
+  <si>
+    <t>When you play this, throw away another Action card from your hand. Use the stronger effect of that card (for free).</t>
+  </si>
+  <si>
+    <t>Extinction Burst</t>
+  </si>
+  <si>
+    <t>Magic Talent</t>
+  </si>
+  <si>
+    <t>Discard a card of any colour. You may play one Dark Matter Device card of the same colour in the DMD Offer this turn as if it were in your hand. That card remains in the offer.</t>
+  </si>
+  <si>
+    <t>When you play this, pay an energy of any colour. Gain a Dark Matter Device card of that colour from the DMD Offer and put it in your discard pile.</t>
+  </si>
+  <si>
+    <t>Dark Matter Lab Contact</t>
+  </si>
+  <si>
+    <t>Learning</t>
+  </si>
+  <si>
+    <t>Influence, Special</t>
+  </si>
+  <si>
+    <t>Influence 2. Once during this turn, you may pay Influence 6 to gain an Advanced Action card from the Advanced Actions Offer to your discard pile.</t>
+  </si>
+  <si>
+    <t>Influence 4. Once during this turn, you may pay Influence 9 to gain an advanced Action card from the Advanced Actions Offer to your hand.</t>
+  </si>
+  <si>
+    <t>Alien Elder Mentor</t>
+  </si>
+  <si>
     <t>Training</t>
   </si>
   <si>
@@ -308,6 +430,18 @@
     <t>Flea Market Contact</t>
   </si>
   <si>
+    <t>Counterattack</t>
+  </si>
+  <si>
+    <t>Attack 2. Get an additional Attack 2 for each enemy blocked this turn.</t>
+  </si>
+  <si>
+    <t>Attack 4. Get an additional Attack 3 for each enemy blocked this turn.</t>
+  </si>
+  <si>
+    <t>Kinetic Storage Space Suit</t>
+  </si>
+  <si>
     <t>Ritual Attack</t>
   </si>
   <si>
@@ -332,6 +466,18 @@
     <t>Black Market Contact</t>
   </si>
   <si>
+    <t>Shield Bash</t>
+  </si>
+  <si>
+    <t>Block 3. Counts twice against an attack with Swiftness.</t>
+  </si>
+  <si>
+    <t>Block 5. Counts twice against an attack with Swiftness. Blocked enemy gets Armor -1 for each point of block higher than needed (to a minimum of 1).</t>
+  </si>
+  <si>
+    <t>Recoil Amplifying Space Suit</t>
+  </si>
+  <si>
     <t>Temporal Portal</t>
   </si>
   <si>
@@ -345,6 +491,81 @@
   </si>
   <si>
     <t>Spacetime Bender</t>
+  </si>
+  <si>
+    <t>Spell Forge</t>
+  </si>
+  <si>
+    <t>Gain one battery to yoyr Inventory of the same colour as one of the cards in the Dark Matter Device offer.</t>
+  </si>
+  <si>
+    <t>Gain two batteries to your Inventory of the same colours as two different cards in the Dark Matter Device Offer.</t>
+  </si>
+  <si>
+    <t>Battery Warehouse Contact</t>
+  </si>
+  <si>
+    <t>Chivalry</t>
+  </si>
+  <si>
+    <t>Attack 3, or Attack 2 and Reputation +1 for each enemy defeated by this atack.</t>
+  </si>
+  <si>
+    <t>Attack 6, or Attack 4 and Reputation +1 and Fame +1 for each enemy defeated by this attack.</t>
+  </si>
+  <si>
+    <t>Alien Combat Ethics Manual</t>
+  </si>
+  <si>
+    <t>Peaceful Moment</t>
+  </si>
+  <si>
+    <t>Influence, Action</t>
+  </si>
+  <si>
+    <t>Influence 3. You may play this as your action for the turn: if you do, you may get Heal 1 for each 2 Influence spent</t>
+  </si>
+  <si>
+    <t>Influence 6. You may play this as your action for the turn: if you do, you may get Heal 1 for each 2 Influence you spend and/or refresh a Unit by paying 2 Influence per level of the Unit.</t>
+  </si>
+  <si>
+    <t>Regeneration Chamber</t>
+  </si>
+  <si>
+    <t>Dodge And Weave</t>
+  </si>
+  <si>
+    <t>Reduce one enemy attack by 2. Gain Attack 1 in the Attack phase if you did not add any Wounds to your hand in the previous combat phases.</t>
+  </si>
+  <si>
+    <t>Reduce one enemy Attack by 4 or two attacks of one or two enemies by 2. Gain Attack 2 in the Attack phase if you did not add any Wounds to your hand in the previous combat phases.</t>
+  </si>
+  <si>
+    <t>Predictive Combat HUD</t>
+  </si>
+  <si>
+    <t>Stout Resolve</t>
+  </si>
+  <si>
+    <t>Move 2, Influence 2, Attack 2, or Block 2. You may discard a Wound to increase the effect by 1.</t>
+  </si>
+  <si>
+    <t>Move 3, Influence 3, Attack or Block 3. You may discard any number of cards, including one Wound, to increase the effect by 2 for each.</t>
+  </si>
+  <si>
+    <t>Artificial Adrenal Glands</t>
+  </si>
+  <si>
+    <t>Force Of Nature</t>
+  </si>
+  <si>
+    <t>Chosen Unit gains Physical resistance this combat</t>
+  </si>
+  <si>
+    <t>Siege Attack 3 or Block 6</t>
+  </si>
+  <si>
+    <t>Mouldable Carbyne</t>
   </si>
   <si>
     <t>Mountain Lore</t>
@@ -458,16 +679,16 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="bottomLeft" activeCell="J27" activeCellId="0" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.2448979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.7908163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -604,6 +825,24 @@
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
+      <c r="B6" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="H6" s="0" t="s">
         <v>14</v>
       </c>
@@ -613,7 +852,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>31</v>
@@ -622,13 +861,13 @@
         <v>16</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H7" s="0" t="s">
         <v>14</v>
@@ -639,22 +878,22 @@
         <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>21</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>14</v>
@@ -664,6 +903,24 @@
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
+      <c r="B9" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>48</v>
+      </c>
       <c r="H9" s="0" t="s">
         <v>14</v>
       </c>
@@ -673,22 +930,22 @@
         <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>14</v>
@@ -698,6 +955,24 @@
       <c r="A11" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="B11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>57</v>
+      </c>
       <c r="H11" s="0" t="s">
         <v>14</v>
       </c>
@@ -707,22 +982,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>21</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="H12" s="0" t="s">
         <v>14</v>
@@ -733,22 +1008,22 @@
         <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>26</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="H13" s="0" t="s">
         <v>14</v>
@@ -759,22 +1034,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="H14" s="0" t="s">
         <v>14</v>
@@ -783,6 +1058,24 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>14</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>75</v>
       </c>
       <c r="H15" s="0" t="s">
         <v>14</v>
@@ -793,22 +1086,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="H16" s="0" t="s">
         <v>14</v>
@@ -819,22 +1112,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>26</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="H17" s="0" t="s">
         <v>14</v>
@@ -845,7 +1138,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>31</v>
@@ -854,13 +1147,13 @@
         <v>10</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="H18" s="0" t="s">
         <v>14</v>
@@ -871,22 +1164,22 @@
         <v>18</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="H19" s="0" t="s">
         <v>14</v>
@@ -897,22 +1190,22 @@
         <v>19</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>21</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="H20" s="0" t="s">
         <v>14</v>
@@ -922,6 +1215,24 @@
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="B21" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>101</v>
+      </c>
       <c r="H21" s="0" t="s">
         <v>14</v>
       </c>
@@ -931,22 +1242,22 @@
         <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="H22" s="0" t="s">
         <v>14</v>
@@ -957,22 +1268,22 @@
         <v>22</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="H23" s="0" t="s">
         <v>14</v>
@@ -982,6 +1293,24 @@
       <c r="A24" s="0" t="n">
         <v>23</v>
       </c>
+      <c r="B24" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>113</v>
+      </c>
       <c r="H24" s="0" t="s">
         <v>14</v>
       </c>
@@ -991,22 +1320,22 @@
         <v>24</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>26</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="H25" s="0" t="s">
         <v>14</v>
@@ -1016,6 +1345,24 @@
       <c r="A26" s="0" t="n">
         <v>25</v>
       </c>
+      <c r="B26" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>121</v>
+      </c>
       <c r="H26" s="0" t="s">
         <v>14</v>
       </c>
@@ -1024,6 +1371,24 @@
       <c r="A27" s="0" t="n">
         <v>26</v>
       </c>
+      <c r="B27" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>125</v>
+      </c>
       <c r="H27" s="0" t="s">
         <v>14</v>
       </c>
@@ -1032,6 +1397,24 @@
       <c r="A28" s="0" t="n">
         <v>27</v>
       </c>
+      <c r="B28" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>130</v>
+      </c>
       <c r="H28" s="0" t="s">
         <v>14</v>
       </c>
@@ -1041,22 +1424,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>26</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>92</v>
+        <v>132</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>93</v>
+        <v>133</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>94</v>
+        <v>134</v>
       </c>
       <c r="H29" s="0" t="s">
         <v>14</v>
@@ -1066,6 +1449,24 @@
       <c r="A30" s="0" t="n">
         <v>29</v>
       </c>
+      <c r="B30" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>138</v>
+      </c>
       <c r="H30" s="0" t="s">
         <v>14</v>
       </c>
@@ -1075,7 +1476,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>95</v>
+        <v>139</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>31</v>
@@ -1084,13 +1485,13 @@
         <v>10</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>96</v>
+        <v>140</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>97</v>
+        <v>141</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>98</v>
+        <v>142</v>
       </c>
       <c r="H31" s="0" t="s">
         <v>14</v>
@@ -1101,22 +1502,22 @@
         <v>31</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>99</v>
+        <v>143</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="D32" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>100</v>
+        <v>144</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>101</v>
+        <v>145</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="H32" s="0" t="s">
         <v>14</v>
@@ -1126,6 +1527,24 @@
       <c r="A33" s="0" t="n">
         <v>32</v>
       </c>
+      <c r="B33" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>150</v>
+      </c>
       <c r="H33" s="0" t="s">
         <v>14</v>
       </c>
@@ -1135,22 +1554,22 @@
         <v>33</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>103</v>
+        <v>151</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="D34" s="0" t="s">
         <v>16</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>106</v>
+        <v>154</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>107</v>
+        <v>155</v>
       </c>
       <c r="H34" s="0" t="s">
         <v>14</v>
@@ -1160,6 +1579,24 @@
       <c r="A35" s="0" t="n">
         <v>34</v>
       </c>
+      <c r="B35" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>159</v>
+      </c>
       <c r="H35" s="0" t="s">
         <v>14</v>
       </c>
@@ -1168,6 +1605,24 @@
       <c r="A36" s="0" t="n">
         <v>35</v>
       </c>
+      <c r="B36" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>163</v>
+      </c>
       <c r="H36" s="0" t="s">
         <v>14</v>
       </c>
@@ -1176,6 +1631,24 @@
       <c r="A37" s="0" t="n">
         <v>36</v>
       </c>
+      <c r="B37" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>168</v>
+      </c>
       <c r="H37" s="0" t="s">
         <v>14</v>
       </c>
@@ -1184,6 +1657,24 @@
       <c r="A38" s="0" t="n">
         <v>37</v>
       </c>
+      <c r="B38" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>172</v>
+      </c>
       <c r="H38" s="0" t="s">
         <v>14</v>
       </c>
@@ -1192,6 +1683,24 @@
       <c r="A39" s="0" t="n">
         <v>38</v>
       </c>
+      <c r="B39" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>176</v>
+      </c>
       <c r="H39" s="0" t="s">
         <v>14</v>
       </c>
@@ -1200,6 +1709,24 @@
       <c r="A40" s="0" t="n">
         <v>39</v>
       </c>
+      <c r="B40" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>180</v>
+      </c>
       <c r="H40" s="0" t="s">
         <v>14</v>
       </c>
@@ -1209,22 +1736,22 @@
         <v>40</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>108</v>
+        <v>181</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>26</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>109</v>
+        <v>182</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>110</v>
+        <v>183</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="H41" s="0" t="s">
         <v>14</v>
@@ -1302,7 +1829,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1330,7 +1857,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Added some DMD Cards
</commit_message>
<xml_diff>
--- a/Cards/Advanced Action Cards/AdvancedActions.xlsx
+++ b/Cards/Advanced Action Cards/AdvancedActions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="968" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,6 +17,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$1:$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Sheet1!$1:$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Sheet1!$1:$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">Sheet1!$1:$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -677,18 +678,21 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J27" activeCellId="0" sqref="J27"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.719387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1829,7 +1833,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1857,7 +1861,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>